<commit_message>
Se agrega 'Subsidio al empleo'
</commit_message>
<xml_diff>
--- a/src/assets/conceptos.xlsx
+++ b/src/assets/conceptos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cesariux23\python\TIMBRADO BASE 2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cencarnacion\develop\timbrado\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -144,34 +144,13 @@
     <t>NoMovimiento</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Importe</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Gravado</t>
-    </r>
+    <t>ImporteGravado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -242,7 +221,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -347,7 +325,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -373,6 +351,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -777,7 +758,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -837,7 +818,7 @@
       <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="11" t="s">
         <v>38</v>
       </c>
       <c r="H2" s="7" t="s">

</xml_diff>